<commit_message>
Integration completed - Verison1
</commit_message>
<xml_diff>
--- a/Ariba Error Report_Dispatcher/Data/Config.xlsx
+++ b/Ariba Error Report_Dispatcher/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubSai\Ariba-Error-Report\Ariba Error Report_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35ADE12-0D65-4377-B70D-49505600764F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B3969E-B41C-43B9-A020-D44429D8C97A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="97">
   <si>
     <t>Name</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -159,14 +156,173 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
+    <t>Ariba Error Report</t>
+  </si>
+  <si>
+    <t>Dev</t>
+  </si>
+  <si>
+    <t>Ariba Error Report_Disptacher</t>
+  </si>
+  <si>
+    <t>Ariba_Credentials</t>
+  </si>
+  <si>
+    <t>https://service.ariba.com/Supplier.aw</t>
+  </si>
+  <si>
+    <t>Stores the login credentials of Ariba portal</t>
+  </si>
+  <si>
+    <t>Ariba supplier portal URL</t>
+  </si>
+  <si>
+    <t>WaitPeriod</t>
+  </si>
+  <si>
+    <t>AribaPortal</t>
+  </si>
+  <si>
+    <t>AribaLoginCredentails</t>
+  </si>
+  <si>
+    <t>Tcode</t>
+  </si>
+  <si>
+    <t>SAP_Language</t>
+  </si>
+  <si>
+    <t>EN</t>
+  </si>
+  <si>
+    <t>SAPFile_Location</t>
+  </si>
+  <si>
+    <t>C:\Program Files (x86)\SAP\FrontEnd\SAPgui\saplogon.exe</t>
+  </si>
+  <si>
+    <t>VariableLogonText</t>
+  </si>
+  <si>
+    <t>Variable Logon</t>
+  </si>
+  <si>
+    <t>SAP_server</t>
+  </si>
+  <si>
+    <t>ERP</t>
+  </si>
+  <si>
+    <t>SAP_Credentials</t>
+  </si>
+  <si>
+    <t>SAP_Client</t>
+  </si>
+  <si>
+    <t>Transaction code of SAP</t>
+  </si>
+  <si>
+    <t>WE05</t>
+  </si>
+  <si>
+    <t>SAP Language</t>
+  </si>
+  <si>
+    <t>Application location of SAP</t>
+  </si>
+  <si>
+    <t>Logon text of SAP</t>
+  </si>
+  <si>
+    <t>Server name of SAP</t>
+  </si>
+  <si>
+    <t>Stores the login credentials of SAP</t>
+  </si>
+  <si>
+    <t>Client number of SAP</t>
+  </si>
+  <si>
+    <t>DownloadPath</t>
+  </si>
+  <si>
+    <t>AribaDownloadPath</t>
+  </si>
+  <si>
+    <t>SegmentNumber</t>
+  </si>
+  <si>
+    <t>WE05FileName</t>
+  </si>
+  <si>
+    <t>WE05.xlsx</t>
+  </si>
+  <si>
+    <t>AribaSegmentNumber</t>
+  </si>
+  <si>
+    <t>ColumnListToAdd</t>
+  </si>
+  <si>
+    <t>AribaColumnList</t>
+  </si>
+  <si>
+    <t>WE05InputSheet</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
+  </si>
+  <si>
+    <t>WE05OutputSheet</t>
+  </si>
+  <si>
+    <t>Sheet2</t>
+  </si>
+  <si>
+    <t>AribaFileName</t>
+  </si>
+  <si>
+    <t>Ariba Report.csv</t>
+  </si>
+  <si>
+    <t>SuccessEmail</t>
+  </si>
+  <si>
+    <t>ExceptionEmail</t>
+  </si>
+  <si>
+    <t>CcEmail</t>
+  </si>
+  <si>
+    <t>SucessEmailBody</t>
+  </si>
+  <si>
+    <t>Document numbers uploaded sucessfully into Queue</t>
+  </si>
+  <si>
+    <t>CcEmail_Ariba</t>
+  </si>
+  <si>
+    <t>ExceptionEmail_Ariba</t>
+  </si>
+  <si>
+    <t>SuccessEmail_Ariba</t>
+  </si>
+  <si>
+    <t>ApplicationID</t>
+  </si>
+  <si>
+    <t>SecretID</t>
+  </si>
+  <si>
+    <t>TenantID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -190,6 +346,17 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -208,10 +375,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -221,9 +389,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{6147BD5F-F114-492E-8DDB-C885FEF17617}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -538,7 +715,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -585,22 +762,24 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -609,10 +788,10 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1619,8 +1798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1673,18 +1852,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1708,7 +1887,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1730,7 +1909,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1741,7 +1920,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1752,86 +1931,232 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="6">
+        <v>400</v>
+      </c>
+      <c r="C27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A28" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A30" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A32" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A34" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -2782,7 +3107,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2800,7 +3127,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2828,13 +3155,83 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3830,5 +4227,6 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
for Go-Live controlled testing
</commit_message>
<xml_diff>
--- a/Ariba Error Report_Dispatcher/Data/Config.xlsx
+++ b/Ariba Error Report_Dispatcher/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubSai\Ariba-Error-Report\Ariba Error Report_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8794FBFC-9EAA-4FF8-81D9-86B6FAEBAAE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891A4A83-AFFD-4E9B-9C0F-62F706DD4BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="99">
   <si>
     <t>Name</t>
   </si>
@@ -316,6 +316,12 @@
   </si>
   <si>
     <t>UAT</t>
+  </si>
+  <si>
+    <t>ExportScript</t>
+  </si>
+  <si>
+    <t>Script\Export.vbs</t>
   </si>
 </sst>
 </file>
@@ -1798,8 +1804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2143,7 +2149,14 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A35" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" t="s">
+        <v>98</v>
+      </c>
+    </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3107,7 +3120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Published for Go live Performer 1.0.1 Dispatcher 1.0.1
</commit_message>
<xml_diff>
--- a/Ariba Error Report_Dispatcher/Data/Config.xlsx
+++ b/Ariba Error Report_Dispatcher/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubSai\Ariba-Error-Report\Ariba Error Report_Dispatcher\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubAnkush\Ariba-Error-Report\Ariba Error Report_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891A4A83-AFFD-4E9B-9C0F-62F706DD4BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D988050B-4557-499B-901D-1B6BAD7A7EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -315,13 +315,13 @@
     <t>TenantID</t>
   </si>
   <si>
-    <t>UAT</t>
-  </si>
-  <si>
     <t>ExportScript</t>
   </si>
   <si>
     <t>Script\Export.vbs</t>
+  </si>
+  <si>
+    <t>Prod</t>
   </si>
 </sst>
 </file>
@@ -721,15 +721,15 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -777,19 +777,19 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="29">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1804,16 +1804,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1850,7 +1850,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1975,7 +1975,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -2151,10 +2151,10 @@
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
       <c r="A35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
         <v>97</v>
-      </c>
-      <c r="B35" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3120,16 +3120,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.90625" customWidth="1"/>
-    <col min="2" max="2" width="30.08984375" customWidth="1"/>
-    <col min="3" max="3" width="60.36328125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.42578125" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3176,7 +3176,7 @@
         <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -3187,7 +3187,7 @@
         <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -3198,7 +3198,7 @@
         <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -3209,7 +3209,7 @@
         <v>92</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
@@ -3220,7 +3220,7 @@
         <v>91</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -3231,7 +3231,7 @@
         <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -3242,7 +3242,7 @@
         <v>93</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
published for Go live
</commit_message>
<xml_diff>
--- a/Ariba Error Report_Dispatcher/Data/Config.xlsx
+++ b/Ariba Error Report_Dispatcher/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubAnkush\Ariba-Error-Report\Ariba Error Report_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D988050B-4557-499B-901D-1B6BAD7A7EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82294C5D-97FC-4634-A1A2-6BE867E58761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -1804,8 +1804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2013,7 +2013,7 @@
         <v>49</v>
       </c>
       <c r="B20">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
@@ -3120,7 +3120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated the package versions
</commit_message>
<xml_diff>
--- a/Ariba Error Report_Dispatcher/Data/Config.xlsx
+++ b/Ariba Error Report_Dispatcher/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubSai\Ariba-Error-Report\Ariba Error Report_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891A4A83-AFFD-4E9B-9C0F-62F706DD4BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670A7A40-4364-40B4-B627-6388CFC231F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -315,13 +315,13 @@
     <t>TenantID</t>
   </si>
   <si>
-    <t>UAT</t>
-  </si>
-  <si>
     <t>ExportScript</t>
   </si>
   <si>
     <t>Script\Export.vbs</t>
+  </si>
+  <si>
+    <t>Dev</t>
   </si>
 </sst>
 </file>
@@ -721,7 +721,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -782,7 +782,7 @@
         <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>31</v>
@@ -1804,7 +1804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -2151,10 +2151,10 @@
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
       <c r="A35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
         <v>97</v>
-      </c>
-      <c r="B35" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3120,8 +3120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3176,7 +3176,7 @@
         <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
@@ -3187,7 +3187,7 @@
         <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -3198,7 +3198,7 @@
         <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -3209,7 +3209,7 @@
         <v>92</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
@@ -3220,7 +3220,7 @@
         <v>91</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -3231,7 +3231,7 @@
         <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -3242,7 +3242,7 @@
         <v>93</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
navigate issue fixed and published for UAT
</commit_message>
<xml_diff>
--- a/Ariba Error Report_Dispatcher/Data/Config.xlsx
+++ b/Ariba Error Report_Dispatcher/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubSai\Ariba-Error-Report\Ariba Error Report_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A678F04A-FFB8-49D7-9EFF-2CD3C9F0A93D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB69B42-6687-4AF6-A09F-3938BA424C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -724,7 +724,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1805,8 +1805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3128,8 +3128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3183,7 +3183,7 @@
       <c r="B2" t="s">
         <v>71</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>99</v>
       </c>
     </row>
@@ -3194,7 +3194,7 @@
       <c r="B3" t="s">
         <v>75</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>99</v>
       </c>
     </row>
@@ -3205,7 +3205,7 @@
       <c r="B4" t="s">
         <v>77</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>99</v>
       </c>
     </row>
@@ -3216,7 +3216,7 @@
       <c r="B5" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>99</v>
       </c>
     </row>
@@ -3227,7 +3227,7 @@
       <c r="B6" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>99</v>
       </c>
     </row>
@@ -3238,7 +3238,7 @@
       <c r="B7" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>99</v>
       </c>
     </row>
@@ -3249,7 +3249,7 @@
       <c r="B8" t="s">
         <v>92</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>